<commit_message>
added assignee column in issue tracker
</commit_message>
<xml_diff>
--- a/MyCart/IssueTracker.xlsx
+++ b/MyCart/IssueTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF3C4FF-C6AD-4EA1-A120-39FCD0A9E511}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCD2C00-39BC-4644-B32F-211A1603DFFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Isues" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Isues!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Isues!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
   <si>
     <t>Title</t>
   </si>
@@ -199,6 +199,39 @@
   <si>
     <t>Story Number</t>
   </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>MC-106</t>
+  </si>
+  <si>
+    <t>MC-107</t>
+  </si>
+  <si>
+    <t>MC-108</t>
+  </si>
+  <si>
+    <t>MC-109</t>
+  </si>
+  <si>
+    <t>MC-110</t>
+  </si>
+  <si>
+    <t>MC-111</t>
+  </si>
+  <si>
+    <t>MC-112</t>
+  </si>
+  <si>
+    <t>MC-113</t>
+  </si>
+  <si>
+    <t>MC-114</t>
+  </si>
+  <si>
+    <t>MC-115</t>
+  </si>
 </sst>
 </file>
 
@@ -265,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -301,11 +334,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -342,6 +386,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +680,8 @@
     <col min="3" max="3" width="58.28515625" customWidth="1"/>
     <col min="4" max="4" width="82.7109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
@@ -654,7 +700,10 @@
       <c r="E1" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -674,7 +723,7 @@
       <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -694,10 +743,9 @@
       <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="1"/>
       <c r="H3" s="2"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -17092,7 +17140,7 @@
       <c r="E4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -17112,7 +17160,7 @@
       <c r="E5" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -17132,7 +17180,7 @@
       <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -17152,13 +17200,13 @@
       <c r="E7" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:16384" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>22</v>
@@ -17172,13 +17220,13 @@
       <c r="E8" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>22</v>
@@ -17192,13 +17240,13 @@
       <c r="E9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>22</v>
@@ -17212,13 +17260,13 @@
       <c r="E10" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>22</v>
@@ -17232,13 +17280,13 @@
       <c r="E11" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>22</v>
@@ -17252,13 +17300,13 @@
       <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>22</v>
@@ -17272,13 +17320,13 @@
       <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>22</v>
@@ -17292,13 +17340,13 @@
       <c r="E14" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>22</v>
@@ -17312,13 +17360,13 @@
       <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>30</v>
@@ -17330,13 +17378,13 @@
       <c r="E16" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>30</v>
@@ -17350,24 +17398,24 @@
       <c r="E17" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="7"/>
       <c r="C18" s="3"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="7"/>
       <c r="C19" s="3"/>
       <c r="D19" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F17" xr:uid="{57F34010-D32E-4D23-ACCD-B445CCA19287}"/>
+  <autoFilter ref="A1:G1" xr:uid="{D4E8A060-A8BA-4964-B373-3D4B8C605788}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added MyCart Database Design document and updated issue tracker
</commit_message>
<xml_diff>
--- a/MyCart/IssueTracker.xlsx
+++ b/MyCart/IssueTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCD2C00-39BC-4644-B32F-211A1603DFFA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D51B486-B4E8-46C2-B0DB-F88BA3BD7FFE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Isues" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Isues!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Isues!$A$1:$G$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>Title</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>database</t>
   </si>
   <si>
     <t>Design Documentation for databse schema and Tables</t>
@@ -103,13 +100,7 @@
 Register button</t>
   </si>
   <si>
-    <t>user manamgement</t>
-  </si>
-  <si>
     <t>MC-105</t>
-  </si>
-  <si>
-    <t>api</t>
   </si>
   <si>
     <t>create end point for create user</t>
@@ -127,13 +118,7 @@
     <t>create my-cart-api repo and initial api solution</t>
   </si>
   <si>
-    <t>create empty repo and solution fro api and commit</t>
-  </si>
-  <si>
     <t>create end point for create product category</t>
-  </si>
-  <si>
-    <t>product manamgement</t>
   </si>
   <si>
     <t>it takes the category name and product details create</t>
@@ -182,16 +167,10 @@
     <t>it returns the all products</t>
   </si>
   <si>
-    <t>my-cart-common</t>
-  </si>
-  <si>
     <t>Sprint</t>
   </si>
   <si>
     <t>BackLog</t>
-  </si>
-  <si>
-    <t>Ready</t>
   </si>
   <si>
     <t>None</t>
@@ -231,6 +210,36 @@
   </si>
   <si>
     <t>MC-115</t>
+  </si>
+  <si>
+    <t>create repo and Test End point for api and commit</t>
+  </si>
+  <si>
+    <t>Sprint1</t>
+  </si>
+  <si>
+    <t>Inprogress</t>
+  </si>
+  <si>
+    <t>Lok</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>User Manamgement</t>
+  </si>
+  <si>
+    <t>Api</t>
+  </si>
+  <si>
+    <t>Product Manamgement</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -669,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,11 +691,12 @@
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>2</v>
@@ -698,10 +708,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>3</v>
@@ -709,42 +719,48 @@
     </row>
     <row r="2" spans="1:16384" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>6</v>
+      <c r="E2" t="s">
+        <v>56</v>
       </c>
-      <c r="E2" t="s">
-        <v>47</v>
+      <c r="F2" t="s">
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:16384" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
+      <c r="E3" t="s">
+        <v>56</v>
       </c>
-      <c r="E3" t="s">
-        <v>47</v>
+      <c r="F3" t="s">
+        <v>58</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="1"/>
@@ -17126,280 +17142,280 @@
     </row>
     <row r="4" spans="1:16384" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:16384" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16384" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16384" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:16384" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -17415,7 +17431,21 @@
       <c r="D19" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{D4E8A060-A8BA-4964-B373-3D4B8C605788}"/>
+  <autoFilter ref="A1:G17" xr:uid="{D4E8A060-A8BA-4964-B373-3D4B8C605788}"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{ED0195D6-DADA-4082-A080-6A55B5BCB05A}">
+      <formula1>"None, Ready, Inprogress, Done"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{8D1CB073-BE8F-49D1-941F-E0709F58D50E}">
+      <formula1>"Lok, Varma"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{F50B2ED2-76B3-448B-995C-0CDF53A53577}">
+      <formula1>"BackLog, Sprint1,Sprint2,Sprint3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{81F950E4-EEEA-4893-9906-96C6A7C80FD8}">
+      <formula1>"Database, Common, User Manamgement,Api,Product Manamgement"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>